<commit_message>
fixes final and ready to test
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="COOLING" sheetId="2" r:id="rId3"/>
     <sheet name="ELECTRICITY" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -802,7 +802,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D8"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,421 +1361,555 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="26">
         <v>0</v>
       </c>
-      <c r="D2" s="11">
+      <c r="E2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="18">
+      <c r="F2" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="3">
         <f>1.3*1.15</f>
         <v>1.4949999999999999</v>
       </c>
-      <c r="D3" s="3">
+      <c r="F3" s="3">
         <f>1.15*0.0886</f>
         <v>0.10188999999999999</v>
       </c>
-      <c r="E3" s="18">
+      <c r="G3" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="3">
         <f>1.68*1.15/0.8</f>
         <v>2.4149999999999996</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <f>1.15*0.12/0.8</f>
         <v>0.17249999999999996</v>
       </c>
-      <c r="E4" s="18">
+      <c r="G4" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0.8</v>
+      </c>
+      <c r="E5" s="3">
         <f>1.22*1.15</f>
         <v>1.4029999999999998</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
         <f>1.15*0.0869</f>
         <v>9.9934999999999996E-2</v>
       </c>
-      <c r="E5" s="18">
+      <c r="G5" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.9</v>
+      </c>
+      <c r="E6" s="3">
         <f>2.63*0.9*1.15</f>
         <v>2.7220499999999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="F6" s="3">
         <f>1.15*0.0413*0.9</f>
         <v>4.2745500000000006E-2</v>
       </c>
-      <c r="E6" s="18">
+      <c r="G6" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="3">
         <f>0.2773328387*1.15</f>
         <v>0.31893276450499997</v>
       </c>
-      <c r="D7" s="3">
+      <c r="F7" s="3">
         <f>1.15*0.014000495</f>
         <v>1.6100569249999998E-2</v>
       </c>
-      <c r="E7" s="18">
+      <c r="G7" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="27">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
         <f>0.695*1.15</f>
         <v>0.7992499999999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <f>1.15*0.0164</f>
         <v>1.8860000000000002E-2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="G8" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="E9" s="3">
         <f>1.15*0.241</f>
         <v>0.27714999999999995</v>
       </c>
-      <c r="D9" s="3">
+      <c r="F9" s="3">
         <f>1.15*0.0112</f>
         <v>1.2879999999999999E-2</v>
       </c>
-      <c r="E9" s="18">
+      <c r="G9" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="27">
+        <v>2.7</v>
+      </c>
+      <c r="E10" s="3">
         <f>ELECTRICITY!C3*1.15/2.7</f>
         <v>1.120185185185185</v>
       </c>
-      <c r="D10" s="3">
+      <c r="F10" s="3">
         <f>ELECTRICITY!D3*1.15/2.7</f>
         <v>1.759074074074074E-2</v>
       </c>
-      <c r="E10" s="22">
+      <c r="G10" s="22">
         <f>0.2/4</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="27">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
         <f>0.795*1.15</f>
         <v>0.91425000000000001</v>
       </c>
-      <c r="D11" s="3">
+      <c r="F11" s="3">
         <f>1.15*0.0179</f>
         <v>2.0584999999999999E-2</v>
       </c>
-      <c r="E11" s="22">
+      <c r="G11" s="22">
         <f>0.2/4</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="3">
         <v>1.55</v>
       </c>
-      <c r="D12" s="3">
+      <c r="F12" s="3">
         <v>8.6900000000000005E-2</v>
       </c>
-      <c r="E12" s="23">
+      <c r="G12" s="23">
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="3">
+      <c r="F13" s="3">
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="E13" s="18">
+      <c r="G13" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="3">
         <v>1.68</v>
       </c>
-      <c r="D14" s="3">
+      <c r="F14" s="3">
         <v>0.112</v>
       </c>
-      <c r="E14" s="18">
+      <c r="G14" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="3">
         <v>0.64100000000000001</v>
       </c>
-      <c r="D15" s="3">
+      <c r="F15" s="3">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="E15" s="18">
+      <c r="G15" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3">
-        <f>C9*0.8</f>
+      <c r="C16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="3">
+        <f>E9*0.8</f>
         <v>0.22171999999999997</v>
       </c>
-      <c r="D16" s="3">
-        <f>D9*0.8</f>
+      <c r="F16" s="3">
+        <f>F9*0.8</f>
         <v>1.0304000000000001E-2</v>
       </c>
-      <c r="E16" s="18">
+      <c r="G16" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3">
-        <f>C9*0.3+C5*0.7</f>
+      <c r="C17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E9*0.3+E5*0.7</f>
         <v>1.0652449999999998</v>
       </c>
-      <c r="D17" s="3">
-        <f>D9*0.3+D5*0.7</f>
+      <c r="F17" s="3">
+        <f>F9*0.3+F5*0.7</f>
         <v>7.3818499999999981E-2</v>
       </c>
-      <c r="E17" s="18">
+      <c r="G17" s="18">
         <v>0.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="3">
-        <f>C9*0.6+C12*0.4</f>
+      <c r="C18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="3">
+        <f>E9*0.6+E12*0.4</f>
         <v>0.78629000000000004</v>
       </c>
-      <c r="D18" s="3">
-        <f>D9*0.6+D12*0.4</f>
+      <c r="F18" s="3">
+        <f>F9*0.6+F12*0.4</f>
         <v>4.2488000000000005E-2</v>
       </c>
-      <c r="E18" s="18">
+      <c r="G18" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="3">
-        <f>C9*0.6+C13*0.3+C12*0.1</f>
+      <c r="C19" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="3">
+        <f>E9*0.6+E13*0.3+E12*0.1</f>
         <v>0.62129000000000001</v>
       </c>
-      <c r="D19" s="3">
-        <f>D9*0.6+D13*0.3+D12*0.1</f>
+      <c r="F19" s="3">
+        <f>F9*0.6+F13*0.3+F12*0.1</f>
         <v>2.3168000000000001E-2</v>
       </c>
-      <c r="E19" s="18">
+      <c r="G19" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E20" s="3">
         <v>1.2761111111111112</v>
       </c>
-      <c r="D20" s="3">
+      <c r="F20" s="3">
         <v>4.6404444444444443E-2</v>
       </c>
-      <c r="E20" s="18">
+      <c r="G20" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="3">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="D21" s="3">
+      <c r="F21" s="3">
         <v>9.3999999999999997E-4</v>
       </c>
-      <c r="E21" s="18">
+      <c r="G21" s="18">
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="3">
-        <f>(0.43*(C21)+0.28*(ELECTRICITY!C3/2.96)+0.18*0.954+0.11*0)</f>
+      <c r="C22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="E22" s="3">
+        <f>(0.43*(E21)+0.28*(ELECTRICITY!C3/2.96)+0.18*0.954+0.11*0)</f>
         <v>0.44359478378378375</v>
       </c>
-      <c r="D22" s="3">
-        <f>(0.43*(D21)+0.28*(ELECTRICITY!D3/2.96)+0.18*0.0149+0.11*0)</f>
+      <c r="F22" s="3">
+        <f>(0.43*(F21)+0.28*(ELECTRICITY!D3/2.96)+0.18*0.0149+0.11*0)</f>
         <v>6.9929567567567578E-3</v>
       </c>
-      <c r="E22" s="18">
+      <c r="G22" s="18">
         <v>0.08</v>
       </c>
     </row>
@@ -1790,7 +1924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2081,11 +2215,11 @@
         <v>28</v>
       </c>
       <c r="C8" s="21">
-        <f>HEATING!C5/0.4</f>
+        <f>HEATING!E5/0.4</f>
         <v>3.5074999999999994</v>
       </c>
       <c r="D8" s="21">
-        <f>HEATING!D5/0.4</f>
+        <f>HEATING!F5/0.4</f>
         <v>0.24983749999999999</v>
       </c>
       <c r="E8" s="21">

</xml_diff>

<commit_message>
major fixes to fields
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -281,13 +281,13 @@
     <t>DH</t>
   </si>
   <si>
-    <t>FUEL</t>
-  </si>
-  <si>
-    <t>RENEWABLE</t>
-  </si>
-  <si>
     <t>DC</t>
+  </si>
+  <si>
+    <t>BOILER</t>
+  </si>
+  <si>
+    <t>SC</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" s="27">
         <v>0.8</v>
@@ -895,7 +895,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" s="27">
         <v>0.6</v>
@@ -920,7 +920,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" s="27">
         <v>0.8</v>
@@ -970,7 +970,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" s="27">
         <v>0.6</v>
@@ -1020,7 +1020,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="27">
         <v>0.7</v>
@@ -1189,7 +1189,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="27">
         <v>0.6</v>
@@ -1214,7 +1214,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="27">
         <v>0.6</v>
@@ -1364,7 +1364,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1390,7 @@
       <c r="D1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1431,7 +1431,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D3" s="27">
         <v>0.8</v>
@@ -1456,7 +1456,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" s="27">
         <v>0.6</v>
@@ -1481,7 +1481,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" s="27">
         <v>0.8</v>
@@ -1531,12 +1531,12 @@
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" s="27">
         <v>0.6</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="13">
         <f>0.2773328387*1.15</f>
         <v>0.31893276450499997</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="27">
         <v>0.7</v>
@@ -1750,7 +1750,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="27">
         <v>0.6</v>
@@ -1775,12 +1775,12 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="27">
         <v>0.6</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="12">
         <f>E9*0.3+E5*0.7</f>
         <v>1.0652449999999998</v>
       </c>
@@ -1805,7 +1805,7 @@
       <c r="D18" s="27">
         <v>0.6</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="12">
         <f>E9*0.6+E12*0.4</f>
         <v>0.78629000000000004</v>
       </c>
@@ -1830,7 +1830,7 @@
       <c r="D19" s="27">
         <v>0.6</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="12">
         <f>E9*0.6+E13*0.3+E12*0.1</f>
         <v>0.62129000000000001</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="D20" s="27">
         <v>0.6</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="12">
         <v>1.2761111111111112</v>
       </c>
       <c r="F20" s="3">
@@ -1878,7 +1878,7 @@
       <c r="D21" s="27">
         <v>0.6</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="12">
         <v>5.3699999999999998E-2</v>
       </c>
       <c r="F21" s="3">
@@ -1925,7 +1925,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2029,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="14">
         <v>0.15609999999999999</v>
@@ -2050,11 +2050,11 @@
         <v>11</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="14">
         <f>ELECTRICITY!C8/4</f>
-        <v>0.87687499999999985</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="14">
         <f>ELECTRICITY!D8/4</f>
@@ -2215,8 +2215,8 @@
         <v>28</v>
       </c>
       <c r="C8" s="21">
-        <f>HEATING!E5/0.4</f>
-        <v>3.5074999999999994</v>
+        <f>HEATING!D5/0.4</f>
+        <v>2</v>
       </c>
       <c r="D8" s="21">
         <f>HEATING!F5/0.4</f>

</xml_diff>

<commit_message>
fix to multiprocessing problem
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\SIN\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -269,25 +269,49 @@
     <t>district cooling network - air-air</t>
   </si>
   <si>
-    <t>EFF</t>
-  </si>
-  <si>
-    <t>ELECTRICITY</t>
-  </si>
-  <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
     <t>DH</t>
   </si>
   <si>
     <t>DC</t>
   </si>
   <si>
-    <t>BOILER</t>
-  </si>
-  <si>
-    <t>SC</t>
+    <t>source_hs</t>
+  </si>
+  <si>
+    <t>eff_hs</t>
+  </si>
+  <si>
+    <t>source_cs</t>
+  </si>
+  <si>
+    <t>eff_cs</t>
+  </si>
+  <si>
+    <t>eff_el</t>
+  </si>
+  <si>
+    <t>source_el</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>PVT</t>
+  </si>
+  <si>
+    <t>source_dhw</t>
+  </si>
+  <si>
+    <t>eff_dhw</t>
+  </si>
+  <si>
+    <t>FUEL</t>
+  </si>
+  <si>
+    <t>SOLAR</t>
   </si>
 </sst>
 </file>
@@ -802,7 +826,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +834,7 @@
     <col min="1" max="1" width="44.28515625" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" style="18" bestFit="1" customWidth="1"/>
@@ -824,10 +848,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -870,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D3" s="27">
         <v>0.8</v>
@@ -895,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D4" s="27">
         <v>0.6</v>
@@ -920,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D5" s="27">
         <v>0.8</v>
@@ -945,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D6" s="27">
         <v>0.9</v>
@@ -970,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D7" s="27">
         <v>0.6</v>
@@ -995,7 +1019,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D8" s="27">
         <v>4</v>
@@ -1020,7 +1044,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D9" s="27">
         <v>0.7</v>
@@ -1045,17 +1069,17 @@
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D10" s="27">
         <v>2.7</v>
       </c>
       <c r="E10" s="3">
-        <f>ELECTRICITY!C3*1.15/2.7</f>
+        <f>ELECTRICITY!E3*1.15/2.7</f>
         <v>1.120185185185185</v>
       </c>
       <c r="F10" s="3">
-        <f>1.15*ELECTRICITY!D3/2.7</f>
+        <f>1.15*ELECTRICITY!F3/2.7</f>
         <v>1.759074074074074E-2</v>
       </c>
       <c r="G10" s="22">
@@ -1071,7 +1095,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D11" s="27">
         <v>3</v>
@@ -1097,7 +1121,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="27">
         <v>0.6</v>
@@ -1120,7 +1144,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="27">
         <v>0.6</v>
@@ -1143,7 +1167,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="27">
         <v>0.6</v>
@@ -1166,7 +1190,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="27">
         <v>0.6</v>
@@ -1189,7 +1213,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D16" s="27">
         <v>0.6</v>
@@ -1214,7 +1238,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="27">
         <v>0.6</v>
@@ -1239,7 +1263,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" s="27">
         <v>0.6</v>
@@ -1264,7 +1288,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="27">
         <v>0.6</v>
@@ -1289,7 +1313,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="27">
         <v>0.6</v>
@@ -1312,7 +1336,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" s="27">
         <v>0.6</v>
@@ -1335,17 +1359,17 @@
         <v>53</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" s="27">
         <v>0.6</v>
       </c>
       <c r="E22" s="3">
-        <f>(0.43*(E21)+0.28*(ELECTRICITY!C3/2.96)+0.18*0.954+0.11*0)</f>
+        <f>(0.43*(E21)+0.28*(ELECTRICITY!E3/2.96)+0.18*0.954+0.11*0)</f>
         <v>0.44359478378378375</v>
       </c>
       <c r="F22" s="3">
-        <f>(0.43*(F21)+0.28*(ELECTRICITY!D3/2.96)+0.18*0.0149+0.11*0)</f>
+        <f>(0.43*(F21)+0.28*(ELECTRICITY!F3/2.96)+0.18*0.0149+0.11*0)</f>
         <v>6.9929567567567578E-3</v>
       </c>
       <c r="G22" s="18">
@@ -1364,7 +1388,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1412,7 @@
         <v>61</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
@@ -1431,7 +1455,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D3" s="27">
         <v>0.8</v>
@@ -1456,7 +1480,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D4" s="27">
         <v>0.6</v>
@@ -1481,7 +1505,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D5" s="27">
         <v>0.8</v>
@@ -1506,7 +1530,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D6" s="27">
         <v>0.9</v>
@@ -1531,7 +1555,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D7" s="27">
         <v>0.6</v>
@@ -1556,7 +1580,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D8" s="27">
         <v>4</v>
@@ -1581,7 +1605,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D9" s="27">
         <v>0.7</v>
@@ -1606,17 +1630,17 @@
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D10" s="27">
         <v>2.7</v>
       </c>
       <c r="E10" s="3">
-        <f>ELECTRICITY!C3*1.15/2.7</f>
+        <f>ELECTRICITY!E3*1.15/2.7</f>
         <v>1.120185185185185</v>
       </c>
       <c r="F10" s="3">
-        <f>ELECTRICITY!D3*1.15/2.7</f>
+        <f>ELECTRICITY!F3*1.15/2.7</f>
         <v>1.759074074074074E-2</v>
       </c>
       <c r="G10" s="22">
@@ -1632,7 +1656,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D11" s="27">
         <v>3</v>
@@ -1658,7 +1682,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="27">
         <v>0.6</v>
@@ -1681,7 +1705,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="27">
         <v>0.6</v>
@@ -1704,7 +1728,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="27">
         <v>0.6</v>
@@ -1727,7 +1751,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" s="27">
         <v>0.6</v>
@@ -1750,7 +1774,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D16" s="27">
         <v>0.6</v>
@@ -1775,7 +1799,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="27">
         <v>0.6</v>
@@ -1800,7 +1824,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D18" s="27">
         <v>0.6</v>
@@ -1825,7 +1849,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D19" s="27">
         <v>0.6</v>
@@ -1850,7 +1874,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" s="27">
         <v>0.6</v>
@@ -1873,7 +1897,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D21" s="27">
         <v>0.6</v>
@@ -1896,17 +1920,17 @@
         <v>53</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D22" s="27">
         <v>0.6</v>
       </c>
       <c r="E22" s="3">
-        <f>(0.43*(E21)+0.28*(ELECTRICITY!C3/2.96)+0.18*0.954+0.11*0)</f>
+        <f>(0.43*(E21)+0.28*(ELECTRICITY!E3/2.96)+0.18*0.954+0.11*0)</f>
         <v>0.44359478378378375</v>
       </c>
       <c r="F22" s="3">
-        <f>(0.43*(F21)+0.28*(ELECTRICITY!D3/2.96)+0.18*0.0149+0.11*0)</f>
+        <f>(0.43*(F21)+0.28*(ELECTRICITY!F3/2.96)+0.18*0.0149+0.11*0)</f>
         <v>6.9929567567567578E-3</v>
       </c>
       <c r="G22" s="18">
@@ -1922,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,11 +1957,12 @@
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1945,19 +1970,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1967,17 +1995,20 @@
       <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="14">
         <v>0</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1985,20 +2016,23 @@
         <v>8</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="14">
+        <v>67</v>
+      </c>
+      <c r="D3" s="28">
+        <v>2.7</v>
+      </c>
+      <c r="E3" s="14">
         <v>1.120185185185185</v>
       </c>
-      <c r="E3" s="14">
+      <c r="F3" s="14">
         <v>1.759074074074074E-2</v>
       </c>
-      <c r="F3" s="21">
-        <f t="shared" ref="F3:F5" si="0">0.2/2.7</f>
+      <c r="G3" s="21">
+        <f t="shared" ref="G3:G5" si="0">0.2/2.7</f>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -2006,22 +2040,25 @@
         <v>9</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="14">
-        <f>D5*0.8</f>
-        <v>0.12487999999999999</v>
+        <v>67</v>
+      </c>
+      <c r="D4" s="28">
+        <v>3</v>
       </c>
       <c r="E4" s="14">
         <f>E5*0.8</f>
+        <v>0.12487999999999999</v>
+      </c>
+      <c r="F4" s="14">
+        <f>F5*0.8</f>
         <v>1.956260204185213E-3</v>
       </c>
-      <c r="F4" s="21">
+      <c r="G4" s="21">
         <f t="shared" si="0"/>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -2029,20 +2066,23 @@
         <v>10</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D5" s="14">
+        <v>3.2</v>
+      </c>
+      <c r="E5" s="14">
         <v>0.15609999999999999</v>
       </c>
-      <c r="E5" s="14">
+      <c r="F5" s="14">
         <v>2.4453252552315164E-3</v>
       </c>
-      <c r="F5" s="21">
+      <c r="G5" s="21">
         <f t="shared" si="0"/>
         <v>7.407407407407407E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>58</v>
       </c>
@@ -2050,18 +2090,21 @@
         <v>11</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="14">
-        <f>ELECTRICITY!C8/4</f>
+        <v>60</v>
+      </c>
+      <c r="D6" s="28">
+        <v>2.8</v>
+      </c>
+      <c r="E6" s="14">
+        <f>ELECTRICITY!E8/4</f>
         <v>0.5</v>
       </c>
-      <c r="E6" s="14">
-        <f>ELECTRICITY!D8/4</f>
+      <c r="F6" s="14">
+        <f>ELECTRICITY!F8/4</f>
         <v>6.2459374999999998E-2</v>
       </c>
-      <c r="F6" s="14">
-        <f>ELECTRICITY!E8/4</f>
+      <c r="G6" s="14">
+        <f>ELECTRICITY!G8/4</f>
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
@@ -2073,10 +2116,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2127,7 @@
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2092,137 +2135,185 @@
         <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="7">
         <v>0</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E3" s="14">
         <v>2.63</v>
       </c>
-      <c r="D3" s="14">
+      <c r="F3" s="14">
         <v>4.1300000000000003E-2</v>
       </c>
-      <c r="E3" s="21">
+      <c r="G3" s="21">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E4" s="14">
         <v>0.27800000000000002</v>
       </c>
-      <c r="D4" s="14">
+      <c r="F4" s="14">
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="E4" s="24">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="24">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E5" s="14">
         <v>0.222</v>
       </c>
-      <c r="D5" s="14">
+      <c r="F5" s="14">
         <v>1.0800000000000001E-2</v>
       </c>
-      <c r="E5" s="24">
+      <c r="G5" s="24">
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14">
-        <f>C4*0.3+C3*0.7</f>
+      <c r="C6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E6" s="14">
+        <f>E4*0.3+E3*0.7</f>
         <v>1.9243999999999997</v>
       </c>
-      <c r="D6" s="14">
-        <f>D4*0.3+D3*0.7</f>
+      <c r="F6" s="14">
+        <f>F4*0.3+F3*0.7</f>
         <v>3.4970000000000001E-2</v>
       </c>
-      <c r="E6" s="21">
+      <c r="G6" s="21">
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14">
-        <f>C5*0.3+C3*0.7</f>
+      <c r="C7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="14">
+        <f>E5*0.3+E3*0.7</f>
         <v>1.9075999999999997</v>
       </c>
-      <c r="D7" s="14">
-        <f>D5*0.3+D3*0.7</f>
+      <c r="F7" s="14">
+        <f>F5*0.3+F3*0.7</f>
         <v>3.2150000000000005E-2</v>
       </c>
-      <c r="E7" s="21">
+      <c r="G7" s="21">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="21">
         <f>HEATING!D5/0.4</f>
         <v>2</v>
       </c>
-      <c r="D8" s="21">
+      <c r="F8" s="21">
         <f>HEATING!F5/0.4</f>
         <v>0.24983749999999999</v>
       </c>
-      <c r="E8" s="21">
+      <c r="G8" s="21">
         <v>0.27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding lca to optimizaiton
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -155,9 +155,6 @@
     <t>oil-fired boiler</t>
   </si>
   <si>
-    <t>gas-fired boiler</t>
-  </si>
-  <si>
     <t>electrical boiler</t>
   </si>
   <si>
@@ -314,7 +311,61 @@
     <t>reference</t>
   </si>
   <si>
-    <t>KBOB 2019</t>
+    <t>KBOB 2019, costs in USD-2015</t>
+  </si>
+  <si>
+    <t>natural gas-fired boiler</t>
+  </si>
+  <si>
+    <t>bio gas-fired boiler</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>from CEA, costs in USD-2015</t>
+  </si>
+  <si>
+    <t>small GHP</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>Green Electricity</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>Natural gas CHP</t>
+  </si>
+  <si>
+    <t>Bio gas CHP</t>
+  </si>
+  <si>
+    <t>Agricultural Bio gas CHP</t>
+  </si>
+  <si>
+    <t>district heating - bio gas-fired boiler</t>
+  </si>
+  <si>
+    <t>district heating - natural gas-fired boiler</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>district heating - agricultural bio gas-fired boiler</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
   </si>
 </sst>
 </file>
@@ -373,7 +424,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -396,12 +447,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -450,6 +512,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -800,25 +876,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -826,10 +902,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -838,13 +914,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -867,10 +943,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -878,7 +954,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="18">
         <v>0.8</v>
@@ -892,13 +968,14 @@
         <v>0.10188999999999999</v>
       </c>
       <c r="G3" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -906,7 +983,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="18">
         <v>0.6</v>
@@ -920,21 +997,22 @@
         <v>0.17249999999999996</v>
       </c>
       <c r="G4" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H4" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="18">
         <v>0.8</v>
@@ -948,21 +1026,22 @@
         <v>9.9934999999999996E-2</v>
       </c>
       <c r="G5" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="18">
         <v>0.9</v>
@@ -976,21 +1055,21 @@
         <v>4.2745500000000006E-2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="18">
         <v>0.6</v>
@@ -1004,21 +1083,22 @@
         <v>1.6100569249999998E-2</v>
       </c>
       <c r="G7" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="18">
         <v>4</v>
@@ -1032,21 +1112,21 @@
         <v>1.8860000000000002E-2</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="18">
         <v>0.7</v>
@@ -1063,18 +1143,18 @@
         <v>0</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="18">
         <v>2.7</v>
@@ -1088,21 +1168,21 @@
         <v>1.759074074074074E-2</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="18">
         <v>3</v>
@@ -1116,21 +1196,21 @@
         <v>2.0584999999999999E-2</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="18">
         <v>0.6</v>
@@ -1142,21 +1222,22 @@
         <v>8.6900000000000005E-2</v>
       </c>
       <c r="G12" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="18">
         <v>0.6</v>
@@ -1168,21 +1249,22 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="G13" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="18">
         <v>0.6</v>
@@ -1194,21 +1276,22 @@
         <v>0.112</v>
       </c>
       <c r="G14" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="18">
         <v>0.6</v>
@@ -1220,21 +1303,22 @@
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="G15" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="18">
         <v>0.6</v>
@@ -1248,21 +1332,22 @@
         <v>7.3818499999999981E-2</v>
       </c>
       <c r="G16" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="18">
         <v>0.6</v>
@@ -1276,21 +1361,22 @@
         <v>4.2488000000000005E-2</v>
       </c>
       <c r="G17" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="18">
         <v>0.6</v>
@@ -1304,21 +1390,22 @@
         <v>2.3168000000000001E-2</v>
       </c>
       <c r="G18" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="18">
         <v>0.6</v>
@@ -1330,21 +1417,22 @@
         <v>4.6404444444444443E-2</v>
       </c>
       <c r="G19" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="18">
         <v>0.6</v>
@@ -1356,21 +1444,22 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="G20" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="18">
         <v>0.6</v>
@@ -1384,10 +1473,39 @@
         <v>6.9929567567567578E-3</v>
       </c>
       <c r="G21" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="E22">
+        <f>0.339*0.87</f>
+        <v>0.29493000000000003</v>
+      </c>
+      <c r="F22">
+        <f>0.04*0.87</f>
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.44</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1399,25 +1517,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1425,10 +1543,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -1437,13 +1555,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1466,10 +1584,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1477,7 +1595,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="18">
         <v>0.8</v>
@@ -1491,13 +1609,14 @@
         <v>0.10188999999999999</v>
       </c>
       <c r="G3" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1505,7 +1624,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="18">
         <v>0.6</v>
@@ -1519,21 +1638,22 @@
         <v>0.17249999999999996</v>
       </c>
       <c r="G4" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H4" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" s="18">
         <v>0.8</v>
@@ -1547,21 +1667,22 @@
         <v>9.9934999999999996E-2</v>
       </c>
       <c r="G5" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="18">
         <v>0.9</v>
@@ -1575,21 +1696,21 @@
         <v>4.2745500000000006E-2</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="18">
         <v>0.6</v>
@@ -1603,21 +1724,22 @@
         <v>1.6100569249999998E-2</v>
       </c>
       <c r="G7" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="18">
         <v>4</v>
@@ -1631,21 +1753,21 @@
         <v>1.8860000000000002E-2</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="18">
         <v>0.7</v>
@@ -1659,21 +1781,22 @@
         <v>1.2879999999999999E-2</v>
       </c>
       <c r="G9" s="15">
+        <f>0*1.1</f>
         <v>0</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="18">
         <v>2.7</v>
@@ -1687,21 +1810,21 @@
         <v>1.759074074074074E-2</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="18">
         <v>3</v>
@@ -1715,21 +1838,21 @@
         <v>2.0584999999999999E-2</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="18">
         <v>0.6</v>
@@ -1741,21 +1864,22 @@
         <v>8.6900000000000005E-2</v>
       </c>
       <c r="G12" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="18">
         <v>0.6</v>
@@ -1767,21 +1891,22 @@
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="G13" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="18">
         <v>0.6</v>
@@ -1793,21 +1918,22 @@
         <v>0.112</v>
       </c>
       <c r="G14" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" s="18">
         <v>0.6</v>
@@ -1819,21 +1945,22 @@
         <v>3.7699999999999997E-2</v>
       </c>
       <c r="G15" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="18">
         <v>0.6</v>
@@ -1847,21 +1974,22 @@
         <v>7.3818499999999981E-2</v>
       </c>
       <c r="G16" s="15">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="18">
         <v>0.6</v>
@@ -1875,21 +2003,22 @@
         <v>4.2488000000000005E-2</v>
       </c>
       <c r="G17" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="18">
         <v>0.6</v>
@@ -1903,21 +2032,22 @@
         <v>2.3168000000000001E-2</v>
       </c>
       <c r="G18" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="18">
         <v>0.6</v>
@@ -1929,21 +2059,22 @@
         <v>4.6404444444444443E-2</v>
       </c>
       <c r="G19" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="18">
         <v>0.6</v>
@@ -1955,21 +2086,22 @@
         <v>9.3999999999999997E-4</v>
       </c>
       <c r="G20" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D21" s="18">
         <v>0.6</v>
@@ -1983,16 +2115,139 @@
         <v>6.9929567567567578E-3</v>
       </c>
       <c r="G21" s="15">
-        <v>0.08</v>
+        <f>0.08*1.1</f>
+        <v>8.8000000000000009E-2</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="E22">
+        <f>0.339*0.87</f>
+        <v>0.29493000000000003</v>
+      </c>
+      <c r="F22">
+        <f>0.04*0.87</f>
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.44</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23">
+        <f>0.706*3.9</f>
+        <v>2.7533999999999996</v>
+      </c>
+      <c r="F23">
+        <f>0.0153*3.9</f>
+        <v>5.9669999999999994E-2</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24">
+        <f>(0.214 + 0.851) * 0.78</f>
+        <v>0.83069999999999999</v>
+      </c>
+      <c r="F24">
+        <f>(0.0223 + 0.114) * 0.78</f>
+        <v>0.10631400000000001</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25">
+        <f>(0.0703 + 0.156) * 0.78</f>
+        <v>0.176514</v>
+      </c>
+      <c r="F25">
+        <f>(0.00592 + 0.0495) * 0.78</f>
+        <v>4.3227600000000005E-2</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26">
+        <f>(0.0353 + 0.186) * 0.78</f>
+        <v>0.17261399999999999</v>
+      </c>
+      <c r="F26">
+        <f>(0.6 + 2.94) * 0.78</f>
+        <v>2.7612000000000001</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2001,21 +2256,21 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2023,10 +2278,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -2035,13 +2290,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2064,10 +2319,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2075,7 +2330,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="11">
         <v>2.7</v>
@@ -2087,13 +2342,13 @@
         <v>1.759074074074074E-2</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2101,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="11">
         <v>3</v>
@@ -2115,21 +2370,21 @@
         <v>1.956260204185213E-3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6">
         <v>3.2</v>
@@ -2141,22 +2396,22 @@
         <v>2.4453252552315164E-3</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" ref="G5" si="0">0.2/2.7</f>
-        <v>7.407407407407407E-2</v>
+        <f>0.2/2.7*1.1</f>
+        <v>8.1481481481481488E-2</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="11">
         <v>2.8</v>
@@ -2170,11 +2425,11 @@
         <v>6.2459374999999998E-2</v>
       </c>
       <c r="G6" s="14">
-        <f>ELECTRICITY!G6/4</f>
-        <v>6.7500000000000004E-2</v>
+        <f>ELECTRICITY!G6/4*1.1</f>
+        <v>8.1675000000000011E-2</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2185,21 +2440,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2207,10 +2462,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -2219,13 +2474,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2248,18 +2503,18 @@
         <v>0</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="4">
         <v>0.99</v>
@@ -2271,21 +2526,22 @@
         <v>4.1300000000000003E-2</v>
       </c>
       <c r="G3" s="13">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="4">
         <v>0.99</v>
@@ -2300,18 +2556,18 @@
         <v>0</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="4">
         <v>0.99</v>
@@ -2325,21 +2581,22 @@
         <v>3.4970000000000001E-2</v>
       </c>
       <c r="G5" s="13">
-        <v>0.2</v>
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="4">
         <v>0.99</v>
@@ -2353,10 +2610,97 @@
         <v>0.24983749999999999</v>
       </c>
       <c r="G6" s="13">
-        <v>0.27</v>
+        <f>0.27*1.1</f>
+        <v>0.29700000000000004</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="24">
+        <v>3.39E-2</v>
+      </c>
+      <c r="F7" s="24">
+        <v>3.98E-3</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8">
+        <f>2.94*0.78</f>
+        <v>2.2932000000000001</v>
+      </c>
+      <c r="F8">
+        <f>0.186*0.78</f>
+        <v>0.14508000000000001</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9">
+        <f>0.851*0.78</f>
+        <v>0.66378000000000004</v>
+      </c>
+      <c r="F9">
+        <f>0.114*0.78</f>
+        <v>8.8920000000000013E-2</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <f>0.156*0.78</f>
+        <v>0.12168000000000001</v>
+      </c>
+      <c r="F10">
+        <f>0.0495*0.78</f>
+        <v>3.8610000000000005E-2</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to recent database strucuture
fixed interface
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>T25</t>
+  </si>
+  <si>
+    <t>from CEA, costs in USD-2015, except for PEN and CO2, rest are assumptions</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -447,23 +450,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -512,20 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -878,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1481,30 +1459,30 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="18">
         <v>0.8</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <f>0.339*0.87</f>
         <v>0.29493000000000003</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <f>0.04*0.87</f>
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="15">
         <v>0.44</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="17" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1519,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1532,7 +1510,7 @@
     <col min="5" max="5" width="7.453125" customWidth="1"/>
     <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2123,125 +2101,143 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="18">
         <v>0.8</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="6">
         <f>0.339*0.87</f>
         <v>0.29493000000000003</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <f>0.04*0.87</f>
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="15">
         <v>0.44</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="6">
         <f>0.706*3.9</f>
         <v>2.7533999999999996</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <f>0.0153*3.9</f>
         <v>5.9669999999999994E-2</v>
       </c>
       <c r="G23" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H23" s="22" t="s">
-        <v>78</v>
+      <c r="H23" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E24">
+      <c r="D24" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E24" s="6">
         <f>(0.214 + 0.851) * 0.78</f>
         <v>0.83069999999999999</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <f>(0.0223 + 0.114) * 0.78</f>
         <v>0.10631400000000001</v>
       </c>
-      <c r="H24" s="22" t="s">
-        <v>78</v>
+      <c r="G24" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E25">
+      <c r="D25" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E25" s="6">
         <f>(0.0703 + 0.156) * 0.78</f>
         <v>0.176514</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <f>(0.00592 + 0.0495) * 0.78</f>
         <v>4.3227600000000005E-2</v>
       </c>
-      <c r="H25" s="22" t="s">
-        <v>78</v>
+      <c r="G25" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E26">
+      <c r="D26" s="18">
+        <v>0.8</v>
+      </c>
+      <c r="E26" s="6">
         <f>(0.0353 + 0.186) * 0.78</f>
         <v>0.17261399999999999</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="6">
         <f>(0.6 + 2.94) * 0.78</f>
         <v>2.7612000000000001</v>
       </c>
-      <c r="H26" s="22" t="s">
-        <v>78</v>
+      <c r="G26" s="15">
+        <v>0.44</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2440,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2454,7 +2450,7 @@
     <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2480,7 +2476,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2533,7 +2529,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
@@ -2559,7 +2555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -2588,7 +2584,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -2617,91 +2613,123 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="24">
+      <c r="D7" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E7" s="9">
         <v>3.39E-2</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="9">
         <v>3.98E-3</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+      <c r="G7" s="13">
+        <f>0.27*1.1</f>
+        <v>0.29700000000000004</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E8">
+      <c r="D8" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E8" s="9">
         <f>2.94*0.78</f>
         <v>2.2932000000000001</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="9">
         <f>0.186*0.78</f>
         <v>0.14508000000000001</v>
       </c>
-      <c r="H8" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+      <c r="G8" s="13">
+        <f>0.27*1.1</f>
+        <v>0.29700000000000004</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E9" s="9">
         <f>0.851*0.78</f>
         <v>0.66378000000000004</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="9">
         <f>0.114*0.78</f>
         <v>8.8920000000000013E-2</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+      <c r="G9" s="13">
+        <f>0.27*1.1</f>
+        <v>0.29700000000000004</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="E10" s="9">
         <f>0.156*0.78</f>
         <v>0.12168000000000001</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="9">
         <f>0.0495*0.78</f>
         <v>3.8610000000000005E-2</v>
       </c>
-      <c r="H10" s="22" t="s">
-        <v>78</v>
-      </c>
+      <c r="G10" s="13">
+        <f>0.27*1.1</f>
+        <v>0.29700000000000004</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modifications in LCA database
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
     <sheet name="HEATING" sheetId="1" r:id="rId2"/>
     <sheet name="COOLING" sheetId="2" r:id="rId3"/>
     <sheet name="ELECTRICITY" sheetId="3" r:id="rId4"/>
+    <sheet name="FUELS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -369,6 +370,30 @@
   </si>
   <si>
     <t>from CEA, costs in USD-2015, except for PEN and CO2, rest are assumptions</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>from CEA, costs in USD-2015,</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>SOLAR</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Wood</t>
   </si>
 </sst>
 </file>
@@ -455,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -470,9 +495,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,9 +512,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -854,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,13 +885,10 @@
     <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -885,20 +901,11 @@
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -908,110 +915,65 @@
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E2" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>0.8</v>
       </c>
-      <c r="E3" s="6">
-        <f>1.3*1.15</f>
-        <v>1.4949999999999999</v>
-      </c>
-      <c r="F3" s="6">
-        <f>1.15*0.0886</f>
-        <v>0.10188999999999999</v>
-      </c>
-      <c r="G3" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E3" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="6">
-        <f>1.68*1.15/0.8</f>
-        <v>2.4149999999999996</v>
-      </c>
-      <c r="F4" s="6">
-        <f>1.15*0.12/0.8</f>
-        <v>0.17249999999999996</v>
-      </c>
-      <c r="G4" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D4" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.8</v>
       </c>
-      <c r="E5" s="6">
-        <f>1.22*1.15</f>
-        <v>1.4029999999999998</v>
-      </c>
-      <c r="F5" s="6">
-        <f>1.15*0.0869</f>
-        <v>9.9934999999999996E-2</v>
-      </c>
-      <c r="G5" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1021,82 +983,48 @@
       <c r="C6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.9</v>
       </c>
-      <c r="E6" s="6">
-        <f>2.63*0.9*1.15</f>
-        <v>2.7220499999999999</v>
-      </c>
-      <c r="F6" s="6">
-        <f>1.15*0.0413*0.9</f>
-        <v>4.2745500000000006E-2</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E6" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E7" s="11">
-        <f>0.2773328387*1.15</f>
-        <v>0.31893276450499997</v>
-      </c>
-      <c r="F7" s="11">
-        <f>1.15*0.014000495</f>
-        <v>1.6100569249999998E-2</v>
-      </c>
-      <c r="G7" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-      <c r="E8" s="6">
-        <f>0.695*1.15</f>
-        <v>0.7992499999999999</v>
-      </c>
-      <c r="F8" s="6">
-        <f>1.15*0.0164</f>
-        <v>1.8860000000000002E-2</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E8" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1106,25 +1034,14 @@
       <c r="C9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>0.7</v>
       </c>
-      <c r="E9" s="6">
-        <f>1.15*0.241</f>
-        <v>0.27714999999999995</v>
-      </c>
-      <c r="F9" s="6">
-        <f>1.15*0.0112</f>
-        <v>1.2879999999999999E-2</v>
-      </c>
-      <c r="G9" s="15">
-        <v>0</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E9" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1134,25 +1051,14 @@
       <c r="C10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>2.7</v>
       </c>
-      <c r="E10" s="6">
-        <f>ELECTRICITY!E3*1.15/2.7</f>
-        <v>1.120185185185185</v>
-      </c>
-      <c r="F10" s="6">
-        <f>1.15*ELECTRICITY!F3/2.7</f>
-        <v>1.759074074074074E-2</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E10" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1162,25 +1068,14 @@
       <c r="C11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
-        <f>0.795*1.15</f>
-        <v>0.91425000000000001</v>
-      </c>
-      <c r="F11" s="6">
-        <f>1.15*0.0179</f>
-        <v>2.0584999999999999E-2</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E11" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1190,24 +1085,14 @@
       <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.55</v>
-      </c>
-      <c r="F12" s="6">
-        <v>8.6900000000000005E-2</v>
-      </c>
-      <c r="G12" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1217,24 +1102,14 @@
       <c r="C13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="G13" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1244,24 +1119,14 @@
       <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.68</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.112</v>
-      </c>
-      <c r="G14" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1271,24 +1136,14 @@
       <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="F15" s="6">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="G15" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1298,26 +1153,14 @@
       <c r="C16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E16" s="6">
-        <f>E9*0.3+E5*0.7</f>
-        <v>1.0652449999999998</v>
-      </c>
-      <c r="F16" s="6">
-        <f>F9*0.3+F5*0.7</f>
-        <v>7.3818499999999981E-2</v>
-      </c>
-      <c r="G16" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1327,26 +1170,14 @@
       <c r="C17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E17" s="6">
-        <f>E9*0.6+E12*0.4</f>
-        <v>0.78629000000000004</v>
-      </c>
-      <c r="F17" s="6">
-        <f>F9*0.6+F12*0.4</f>
-        <v>4.2488000000000005E-2</v>
-      </c>
-      <c r="G17" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D17" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1356,26 +1187,14 @@
       <c r="C18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E18" s="6">
-        <f>E9*0.6+E13*0.3+E12*0.1</f>
-        <v>0.62129000000000001</v>
-      </c>
-      <c r="F18" s="6">
-        <f>F9*0.6+F13*0.3+F12*0.1</f>
-        <v>2.3168000000000001E-2</v>
-      </c>
-      <c r="G18" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1385,24 +1204,14 @@
       <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1.2761111111111112</v>
-      </c>
-      <c r="F19" s="6">
-        <v>4.6404444444444443E-2</v>
-      </c>
-      <c r="G19" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1412,77 +1221,44 @@
       <c r="C20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E20" s="6">
-        <v>5.3699999999999998E-2</v>
-      </c>
-      <c r="F20" s="6">
-        <v>9.3999999999999997E-4</v>
-      </c>
-      <c r="G20" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D20" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E21" s="6">
-        <f>(0.43*(E20)+0.28*(ELECTRICITY!E3/2.96)+0.18*0.954+0.11*0)</f>
-        <v>0.44359478378378375</v>
-      </c>
-      <c r="F21" s="6">
-        <f>(0.43*(F20)+0.28*(ELECTRICITY!F3/2.96)+0.18*0.0149+0.11*0)</f>
-        <v>6.9929567567567578E-3</v>
-      </c>
-      <c r="G21" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>0.8</v>
       </c>
-      <c r="E22" s="6">
-        <f>0.339*0.87</f>
-        <v>0.29493000000000003</v>
-      </c>
-      <c r="F22" s="6">
-        <f>0.04*0.87</f>
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="H22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1495,10 +1271,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1507,13 +1283,10 @@
     <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.26953125" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1526,20 +1299,11 @@
       <c r="D1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1549,110 +1313,65 @@
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="15">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E2" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <v>0.8</v>
       </c>
-      <c r="E3" s="6">
-        <f>1.3*1.15</f>
-        <v>1.4949999999999999</v>
-      </c>
-      <c r="F3" s="6">
-        <f>1.15*0.0886</f>
-        <v>0.10188999999999999</v>
-      </c>
-      <c r="G3" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E3" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="6">
-        <f>1.68*1.15/0.8</f>
-        <v>2.4149999999999996</v>
-      </c>
-      <c r="F4" s="6">
-        <f>1.15*0.12/0.8</f>
-        <v>0.17249999999999996</v>
-      </c>
-      <c r="G4" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D4" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>0.8</v>
       </c>
-      <c r="E5" s="6">
-        <f>1.22*1.15</f>
-        <v>1.4029999999999998</v>
-      </c>
-      <c r="F5" s="6">
-        <f>1.15*0.0869</f>
-        <v>9.9934999999999996E-2</v>
-      </c>
-      <c r="G5" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1662,54 +1381,31 @@
       <c r="C6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>0.9</v>
       </c>
-      <c r="E6" s="6">
-        <f>2.63*0.9*1.15</f>
-        <v>2.7220499999999999</v>
-      </c>
-      <c r="F6" s="6">
-        <f>1.15*0.0413*0.9</f>
-        <v>4.2745500000000006E-2</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E6" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E7" s="11">
-        <f>0.2773328387*1.15</f>
-        <v>0.31893276450499997</v>
-      </c>
-      <c r="F7" s="6">
-        <f>1.15*0.014000495</f>
-        <v>1.6100569249999998E-2</v>
-      </c>
-      <c r="G7" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1719,25 +1415,14 @@
       <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>4</v>
       </c>
-      <c r="E8" s="6">
-        <f>0.695*1.15</f>
-        <v>0.7992499999999999</v>
-      </c>
-      <c r="F8" s="6">
-        <f>1.15*0.0164</f>
-        <v>1.8860000000000002E-2</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E8" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1747,26 +1432,14 @@
       <c r="C9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>0.7</v>
       </c>
-      <c r="E9" s="6">
-        <f>1.15*0.241</f>
-        <v>0.27714999999999995</v>
-      </c>
-      <c r="F9" s="6">
-        <f>1.15*0.0112</f>
-        <v>1.2879999999999999E-2</v>
-      </c>
-      <c r="G9" s="15">
-        <f>0*1.1</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E9" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1776,25 +1449,14 @@
       <c r="C10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>2.7</v>
       </c>
-      <c r="E10" s="6">
-        <f>ELECTRICITY!E3*1.15/2.7</f>
-        <v>1.120185185185185</v>
-      </c>
-      <c r="F10" s="6">
-        <f>ELECTRICITY!F3*1.15/2.7</f>
-        <v>1.759074074074074E-2</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E10" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1804,25 +1466,14 @@
       <c r="C11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
-        <f>0.795*1.15</f>
-        <v>0.91425000000000001</v>
-      </c>
-      <c r="F11" s="6">
-        <f>1.15*0.0179</f>
-        <v>2.0584999999999999E-2</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E11" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1832,24 +1483,14 @@
       <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.55</v>
-      </c>
-      <c r="F12" s="6">
-        <v>8.6900000000000005E-2</v>
-      </c>
-      <c r="G12" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1859,24 +1500,14 @@
       <c r="C13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="G13" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1886,24 +1517,14 @@
       <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.68</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.112</v>
-      </c>
-      <c r="G14" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1913,24 +1534,14 @@
       <c r="C15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="F15" s="6">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="G15" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1940,26 +1551,14 @@
       <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E16" s="6">
-        <f>E9*0.3+E5*0.7</f>
-        <v>1.0652449999999998</v>
-      </c>
-      <c r="F16" s="6">
-        <f>F9*0.3+F5*0.7</f>
-        <v>7.3818499999999981E-2</v>
-      </c>
-      <c r="G16" s="15">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1969,26 +1568,14 @@
       <c r="C17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E17" s="6">
-        <f>E9*0.6+E12*0.4</f>
-        <v>0.78629000000000004</v>
-      </c>
-      <c r="F17" s="6">
-        <f>F9*0.6+F12*0.4</f>
-        <v>4.2488000000000005E-2</v>
-      </c>
-      <c r="G17" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D17" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1998,26 +1585,14 @@
       <c r="C18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E18" s="6">
-        <f>E9*0.6+E13*0.3+E12*0.1</f>
-        <v>0.62129000000000001</v>
-      </c>
-      <c r="F18" s="6">
-        <f>F9*0.6+F13*0.3+F12*0.1</f>
-        <v>2.3168000000000001E-2</v>
-      </c>
-      <c r="G18" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -2027,24 +1602,14 @@
       <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1.2761111111111112</v>
-      </c>
-      <c r="F19" s="6">
-        <v>4.6404444444444443E-2</v>
-      </c>
-      <c r="G19" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D19" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -2054,53 +1619,31 @@
       <c r="C20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E20" s="6">
-        <v>5.3699999999999998E-2</v>
-      </c>
-      <c r="F20" s="6">
-        <v>9.3999999999999997E-4</v>
-      </c>
-      <c r="G20" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D20" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="18">
-        <v>0.6</v>
-      </c>
-      <c r="E21" s="6">
-        <f>(0.43*(E20)+0.28*(ELECTRICITY!E3/2.96)+0.18*0.954+0.11*0)</f>
-        <v>0.44359478378378375</v>
-      </c>
-      <c r="F21" s="6">
-        <f>(0.43*(F20)+0.28*(ELECTRICITY!F3/2.96)+0.18*0.0149+0.11*0)</f>
-        <v>6.9929567567567578E-3</v>
-      </c>
-      <c r="G21" s="15">
-        <f>0.08*1.1</f>
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -2110,25 +1653,14 @@
       <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="16">
         <v>0.8</v>
       </c>
-      <c r="E22" s="6">
-        <f>0.339*0.87</f>
-        <v>0.29493000000000003</v>
-      </c>
-      <c r="F22" s="6">
-        <f>0.04*0.87</f>
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="H22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -2138,25 +1670,14 @@
       <c r="C23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="6">
-        <f>0.706*3.9</f>
-        <v>2.7533999999999996</v>
-      </c>
-      <c r="F23" s="6">
-        <f>0.0153*3.9</f>
-        <v>5.9669999999999994E-2</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -2166,25 +1687,14 @@
       <c r="C24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="16">
         <v>0.8</v>
       </c>
-      <c r="E24" s="6">
-        <f>(0.214 + 0.851) * 0.78</f>
-        <v>0.83069999999999999</v>
-      </c>
-      <c r="F24" s="6">
-        <f>(0.0223 + 0.114) * 0.78</f>
-        <v>0.10631400000000001</v>
-      </c>
-      <c r="G24" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="H24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -2194,25 +1704,14 @@
       <c r="C25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="16">
         <v>0.8</v>
       </c>
-      <c r="E25" s="6">
-        <f>(0.0703 + 0.156) * 0.78</f>
-        <v>0.176514</v>
-      </c>
-      <c r="F25" s="6">
-        <f>(0.00592 + 0.0495) * 0.78</f>
-        <v>4.3227600000000005E-2</v>
-      </c>
-      <c r="G25" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="H25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
@@ -2222,21 +1721,10 @@
       <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="16">
         <v>0.8</v>
       </c>
-      <c r="E26" s="6">
-        <f>(0.0353 + 0.186) * 0.78</f>
-        <v>0.17261399999999999</v>
-      </c>
-      <c r="F26" s="6">
-        <f>(0.6 + 2.94) * 0.78</f>
-        <v>2.7612000000000001</v>
-      </c>
-      <c r="G26" s="15">
-        <v>0.44</v>
-      </c>
-      <c r="H26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2249,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2261,12 +1749,10 @@
     <col min="2" max="2" width="7.26953125" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2279,20 +1765,11 @@
       <c r="D1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2305,74 +1782,45 @@
       <c r="D2" s="6">
         <v>0</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E2" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>2.7</v>
       </c>
-      <c r="E3" s="6">
-        <v>1.120185185185185</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1.759074074074074E-2</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E3" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="6">
-        <f>E5*0.8</f>
-        <v>0.12487999999999999</v>
-      </c>
-      <c r="F4" s="6">
-        <f>F5*0.8</f>
-        <v>1.956260204185213E-3</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E4" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -2385,46 +1833,24 @@
       <c r="D5" s="6">
         <v>3.2</v>
       </c>
-      <c r="E5" s="6">
-        <v>0.15609999999999999</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2.4453252552315164E-3</v>
-      </c>
-      <c r="G5" s="13">
-        <f>0.2/2.7*1.1</f>
-        <v>8.1481481481481488E-2</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>2.8</v>
       </c>
-      <c r="E6" s="6">
-        <f>ELECTRICITY!E6/4</f>
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="6">
-        <f>ELECTRICITY!F6/4</f>
-        <v>6.2459374999999998E-2</v>
-      </c>
-      <c r="G6" s="14">
-        <f>ELECTRICITY!G6/4*1.1</f>
-        <v>8.1675000000000011E-2</v>
-      </c>
-      <c r="H6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2438,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2469,10 +1895,10 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2495,10 +1921,10 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>0</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2521,11 +1947,11 @@
       <c r="F3" s="6">
         <v>4.1300000000000003E-2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2548,10 +1974,10 @@
       <c r="F4" s="6">
         <v>2.0199999999999999E-2</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <v>0</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2576,11 +2002,11 @@
         <f>F4*0.3+F3*0.7</f>
         <v>3.4970000000000001E-2</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2588,7 +2014,7 @@
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -2597,19 +2023,19 @@
       <c r="D6" s="4">
         <v>0.99</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <f>HEATING!D5/0.4</f>
         <v>2</v>
       </c>
-      <c r="F6" s="9">
-        <f>HEATING!F5/0.4</f>
-        <v>0.24983749999999999</v>
-      </c>
-      <c r="G6" s="13">
+      <c r="F6" s="8" t="e">
+        <f>HEATING!#REF!/0.4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G6" s="12">
         <f>0.27*1.1</f>
         <v>0.29700000000000004</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2617,7 +2043,7 @@
       <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2626,17 +2052,17 @@
       <c r="D7" s="4">
         <v>0.99</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>3.39E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>3.98E-3</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <f>0.27*1.1</f>
         <v>0.29700000000000004</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="15" t="s">
         <v>92</v>
       </c>
       <c r="J7" s="5"/>
@@ -2645,7 +2071,7 @@
       <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -2654,19 +2080,19 @@
       <c r="D8" s="4">
         <v>0.99</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f>2.94*0.78</f>
         <v>2.2932000000000001</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f>0.186*0.78</f>
         <v>0.14508000000000001</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <f>0.27*1.1</f>
         <v>0.29700000000000004</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="15" t="s">
         <v>92</v>
       </c>
       <c r="J8" s="5"/>
@@ -2675,7 +2101,7 @@
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2684,19 +2110,19 @@
       <c r="D9" s="4">
         <v>0.99</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>0.851*0.78</f>
         <v>0.66378000000000004</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <f>0.114*0.78</f>
         <v>8.8920000000000013E-2</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="12">
         <f>0.27*1.1</f>
         <v>0.29700000000000004</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="15" t="s">
         <v>92</v>
       </c>
       <c r="J9" s="5"/>
@@ -2705,7 +2131,7 @@
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -2714,19 +2140,19 @@
       <c r="D10" s="4">
         <v>0.99</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <f>0.156*0.78</f>
         <v>0.12168000000000001</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <f>0.0495*0.78</f>
         <v>3.8610000000000005E-2</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <f>0.27*1.1</f>
         <v>0.29700000000000004</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="15" t="s">
         <v>92</v>
       </c>
       <c r="J10" s="5"/>
@@ -2734,4 +2160,140 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.403</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.6860067999999999E-2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.63</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="E3" s="12">
+        <f>0.2*1.1</f>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
"Fuel" sheet update for both CH and SIN
- updated PEN & CO2 in "Fuel" sheet for various fuels CH (data source: KBOB 2009/1:2016)
- updated PEN & CO2 for natural gas (NG)  in  "Fuel" sheet for SIN (data source: ecoinvent 3.4 market for natural gas, burned in gas motor, for storage, GLO)
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="110">
   <si>
     <t>Description</t>
   </si>
@@ -394,6 +394,33 @@
   </si>
   <si>
     <t>Wood</t>
+  </si>
+  <si>
+    <t>Biogas</t>
+  </si>
+  <si>
+    <t>BIOGAS</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.004/41.005 (average)</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.006 Stückholz (average)</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.009 Biogas</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.002 Erdgas</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.001 Heizöl</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix, costs in USD-2015</t>
   </si>
 </sst>
 </file>
@@ -480,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -524,6 +551,16 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,19 +913,19 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -905,7 +942,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -922,7 +959,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -939,7 +976,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -956,7 +993,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -973,7 +1010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -990,7 +1027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1007,7 +1044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1061,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1041,7 +1078,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1058,7 +1095,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1129,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1109,7 +1146,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1126,7 +1163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1180,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +1214,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1231,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1211,7 +1248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1228,7 +1265,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1245,7 +1282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
@@ -1273,20 +1310,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1340,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1374,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1354,7 +1391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -1371,7 +1408,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1425,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1405,7 +1442,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1422,7 +1459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1439,7 +1476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1456,7 +1493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +1510,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1527,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1524,7 +1561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1541,7 +1578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1558,7 +1595,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1575,7 +1612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1592,7 +1629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1609,7 +1646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1626,7 +1663,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1643,7 +1680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1660,7 +1697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1677,7 +1714,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -1694,7 +1731,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -1711,7 +1748,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
@@ -1743,16 +1780,16 @@
       <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +1823,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1803,7 +1840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1820,7 +1857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1837,7 +1874,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1865,18 +1902,18 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1965,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1942,20 +1979,20 @@
         <v>0.99</v>
       </c>
       <c r="E3" s="6">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="F3" s="6">
-        <v>4.1300000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
@@ -1981,7 +2018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1996,11 +2033,11 @@
       </c>
       <c r="E5" s="6">
         <f>E4*0.3+E3*0.7</f>
-        <v>1.9243999999999997</v>
+        <v>1.8473999999999997</v>
       </c>
       <c r="F5" s="6">
         <f>F4*0.3+F3*0.7</f>
-        <v>3.4970000000000001E-2</v>
+        <v>2.5659999999999999E-2</v>
       </c>
       <c r="G5" s="12">
         <f>0.2*1.1</f>
@@ -2010,7 +2047,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -2039,7 +2076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
@@ -2067,7 +2104,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
@@ -2097,7 +2134,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
@@ -2127,7 +2164,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -2164,19 +2201,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +2234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -2204,19 +2242,20 @@
         <v>69</v>
       </c>
       <c r="C2" s="2">
-        <v>1.403</v>
+        <v>1.06</v>
       </c>
       <c r="D2" s="2">
-        <v>0.1</v>
+        <f>0.228/3.6</f>
+        <v>6.3333333333333339E-2</v>
       </c>
       <c r="E2" s="2">
         <v>1.6860067999999999E-2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
@@ -2224,20 +2263,21 @@
         <v>62</v>
       </c>
       <c r="C3" s="6">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="D3" s="6">
-        <v>4.1300000000000003E-2</v>
+        <f>0.102/3.6</f>
+        <v>2.8333333333333332E-2</v>
       </c>
       <c r="E3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -2257,43 +2297,93 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D5" s="2">
+        <f>0.301/3.6</f>
+        <v>8.3611111111111108E-2</v>
+      </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2">
+        <f>(1.2+1.45)/2</f>
+        <v>1.325</v>
+      </c>
+      <c r="D6" s="2">
+        <f>((0.399+0.439)/2)/3.6</f>
+        <v>0.1163888888888889</v>
+      </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <f>0.027/3.6</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <f>0.13/3.6</f>
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert ""Fuel" sheet update for both CH and SIN"
This reverts commit 714129630cced5ea650676c481bf52750e759138.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -394,33 +394,6 @@
   </si>
   <si>
     <t>Wood</t>
-  </si>
-  <si>
-    <t>Biogas</t>
-  </si>
-  <si>
-    <t>BIOGAS</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.004/41.005 (average)</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.006 Stückholz (average)</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.009 Biogas</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.002 Erdgas</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.001 Heizöl</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix, costs in USD-2015</t>
   </si>
 </sst>
 </file>
@@ -507,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -551,16 +524,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,19 +876,19 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -942,7 +905,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -959,7 +922,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -976,7 +939,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -993,7 +956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -1010,7 +973,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1027,7 +990,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1044,7 +1007,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1061,7 +1024,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1095,7 +1058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1112,7 +1075,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1146,7 +1109,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1163,7 +1126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1180,7 +1143,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1160,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1214,7 +1177,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1231,7 +1194,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1248,7 +1211,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1265,7 +1228,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1282,7 +1245,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
@@ -1310,20 +1273,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1303,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1357,7 +1320,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1374,7 +1337,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1391,7 +1354,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -1408,7 +1371,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1442,7 +1405,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1459,7 +1422,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1476,7 +1439,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1493,7 +1456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1510,7 +1473,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1527,7 +1490,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1544,7 +1507,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1561,7 +1524,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1578,7 +1541,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1595,7 +1558,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1612,7 +1575,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1629,7 +1592,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1646,7 +1609,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1663,7 +1626,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1680,7 +1643,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1697,7 +1660,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1714,7 +1677,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -1731,7 +1694,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -1748,7 +1711,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
@@ -1780,16 +1743,16 @@
       <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1769,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1823,7 +1786,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1840,7 +1803,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1857,7 +1820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1874,7 +1837,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1902,18 +1865,18 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1939,7 +1902,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +1928,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1979,20 +1942,20 @@
         <v>0.99</v>
       </c>
       <c r="E3" s="6">
-        <v>2.52</v>
+        <v>2.63</v>
       </c>
       <c r="F3" s="6">
-        <v>2.8000000000000001E-2</v>
+        <v>4.1300000000000003E-2</v>
       </c>
       <c r="G3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
@@ -2018,7 +1981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -2033,11 +1996,11 @@
       </c>
       <c r="E5" s="6">
         <f>E4*0.3+E3*0.7</f>
-        <v>1.8473999999999997</v>
+        <v>1.9243999999999997</v>
       </c>
       <c r="F5" s="6">
         <f>F4*0.3+F3*0.7</f>
-        <v>2.5659999999999999E-2</v>
+        <v>3.4970000000000001E-2</v>
       </c>
       <c r="G5" s="12">
         <f>0.2*1.1</f>
@@ -2047,7 +2010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -2076,7 +2039,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
@@ -2104,7 +2067,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
@@ -2134,7 +2097,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
@@ -2164,7 +2127,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -2201,20 +2164,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2234,7 +2196,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -2242,20 +2204,19 @@
         <v>69</v>
       </c>
       <c r="C2" s="2">
-        <v>1.06</v>
+        <v>1.403</v>
       </c>
       <c r="D2" s="2">
-        <f>0.228/3.6</f>
-        <v>6.3333333333333339E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="2">
         <v>1.6860067999999999E-2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
@@ -2263,21 +2224,20 @@
         <v>62</v>
       </c>
       <c r="C3" s="6">
-        <v>2.52</v>
+        <v>2.63</v>
       </c>
       <c r="D3" s="6">
-        <f>0.102/3.6</f>
-        <v>2.8333333333333332E-2</v>
+        <v>4.1300000000000003E-2</v>
       </c>
       <c r="E3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -2297,93 +2257,43 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.23</v>
-      </c>
-      <c r="D5" s="2">
-        <f>0.301/3.6</f>
-        <v>8.3611111111111108E-2</v>
-      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="2">
-        <f>(1.2+1.45)/2</f>
-        <v>1.325</v>
-      </c>
-      <c r="D6" s="2">
-        <f>((0.399+0.439)/2)/3.6</f>
-        <v>0.1163888888888889</v>
-      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="D7" s="2">
-        <f>0.027/3.6</f>
-        <v>7.4999999999999997E-3</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="D8" s="2">
-        <f>0.13/3.6</f>
-        <v>3.6111111111111115E-2</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="F7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"Fuel" sheet update for both CH and SIN database
- updated PEN & CO2 in "Fuel" sheet for various fuels CH (data source: KBOB 2009/1:2016)
- updated PEN & CO2 for natural gas (NG) in "Fuel" sheet for SIN (data source: ecoinvent 3.4 market for natural gas, burned in gas motor, for storage, GLO)
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhargava\Documents\GitHub\CEAforArcGIS\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="110">
   <si>
     <t>Description</t>
   </si>
@@ -394,6 +394,33 @@
   </si>
   <si>
     <t>Wood</t>
+  </si>
+  <si>
+    <t>Biogas</t>
+  </si>
+  <si>
+    <t>BIOGAS</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.004/41.005 (average)</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.006 Stückholz (average)</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.009 Biogas</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.002 Erdgas</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.001 Heizöl</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix, costs in USD-2015</t>
   </si>
 </sst>
 </file>
@@ -480,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -524,6 +551,16 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,19 +913,19 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -905,7 +942,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -922,7 +959,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -939,7 +976,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -956,7 +993,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -973,7 +1010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -990,7 +1027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1007,7 +1044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1061,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1041,7 +1078,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
@@ -1058,7 +1095,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1075,7 +1112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1129,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1109,7 +1146,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1126,7 +1163,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1180,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1177,7 +1214,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1231,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1211,7 +1248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1228,7 +1265,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1245,7 +1282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>75</v>
       </c>
@@ -1273,20 +1310,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.26953125" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1340,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1357,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1374,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1354,7 +1391,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -1371,7 +1408,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1388,7 +1425,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1405,7 +1442,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1422,7 +1459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1439,7 +1476,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1456,7 +1493,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1473,7 +1510,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1490,7 +1527,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1524,7 +1561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -1541,7 +1578,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -1558,7 +1595,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
@@ -1575,7 +1612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1592,7 +1629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1609,7 +1646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -1626,7 +1663,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1643,7 +1680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1660,7 +1697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1677,7 +1714,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
@@ -1694,7 +1731,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -1711,7 +1748,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
@@ -1743,16 +1780,16 @@
       <selection activeCell="E1" sqref="E1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +1823,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1803,7 +1840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1820,7 +1857,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -1837,7 +1874,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1865,18 +1902,18 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1965,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -1942,20 +1979,20 @@
         <v>0.99</v>
       </c>
       <c r="E3" s="6">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="F3" s="6">
-        <v>4.1300000000000003E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>39</v>
       </c>
@@ -1981,7 +2018,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -1996,11 +2033,11 @@
       </c>
       <c r="E5" s="6">
         <f>E4*0.3+E3*0.7</f>
-        <v>1.9243999999999997</v>
+        <v>1.8473999999999997</v>
       </c>
       <c r="F5" s="6">
         <f>F4*0.3+F3*0.7</f>
-        <v>3.4970000000000001E-2</v>
+        <v>2.5659999999999999E-2</v>
       </c>
       <c r="G5" s="12">
         <f>0.2*1.1</f>
@@ -2010,7 +2047,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -2039,7 +2076,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>81</v>
       </c>
@@ -2067,7 +2104,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>83</v>
       </c>
@@ -2097,7 +2134,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>84</v>
       </c>
@@ -2127,7 +2164,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -2164,19 +2201,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +2234,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>93</v>
       </c>
@@ -2204,19 +2242,20 @@
         <v>69</v>
       </c>
       <c r="C2" s="2">
-        <v>1.403</v>
+        <v>1.06</v>
       </c>
       <c r="D2" s="2">
-        <v>0.1</v>
+        <f>0.228/3.6</f>
+        <v>6.3333333333333339E-2</v>
       </c>
       <c r="E2" s="2">
         <v>1.6860067999999999E-2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
@@ -2224,20 +2263,21 @@
         <v>62</v>
       </c>
       <c r="C3" s="6">
-        <v>2.63</v>
+        <v>2.52</v>
       </c>
       <c r="D3" s="6">
-        <v>4.1300000000000003E-2</v>
+        <f>0.102/3.6</f>
+        <v>2.8333333333333332E-2</v>
       </c>
       <c r="E3" s="12">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>96</v>
       </c>
@@ -2257,43 +2297,93 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="D5" s="2">
+        <f>0.301/3.6</f>
+        <v>8.3611111111111108E-2</v>
+      </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2">
+        <f>(1.2+1.45)/2</f>
+        <v>1.325</v>
+      </c>
+      <c r="D6" s="2">
+        <f>((0.399+0.439)/2)/3.6</f>
+        <v>0.1163888888888889</v>
+      </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <f>0.027/3.6</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <f>0.13/3.6</f>
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes to lca database based on discussion
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="85">
   <si>
     <t>Description</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Wood</t>
   </si>
   <si>
-    <t>Biogas</t>
-  </si>
-  <si>
     <t>BIOGAS</t>
   </si>
   <si>
@@ -330,19 +327,25 @@
     <t>NATURALGAS</t>
   </si>
   <si>
-    <t>centralized</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Solid Waste</t>
   </si>
   <si>
     <t>WASTE</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>BUILDING</t>
+  </si>
+  <si>
+    <t>DISTRICT</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>Bio Gas</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E19"/>
+      <selection activeCell="D1" sqref="D1:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -877,7 +880,7 @@
         <v>38</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>39</v>
@@ -894,10 +897,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
@@ -915,7 +918,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="13">
         <v>0.8</v>
@@ -933,7 +936,7 @@
         <v>41</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="13">
         <v>0.6</v>
@@ -948,10 +951,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" s="13">
         <v>0.8</v>
@@ -968,8 +971,8 @@
       <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>80</v>
+      <c r="D6" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E6" s="13">
         <v>0.9</v>
@@ -986,8 +989,8 @@
       <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>80</v>
+      <c r="D7" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E7" s="13">
         <v>0.6</v>
@@ -1004,8 +1007,8 @@
       <c r="C8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>80</v>
+      <c r="D8" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E8" s="13">
         <v>4</v>
@@ -1022,8 +1025,8 @@
       <c r="C9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>80</v>
+      <c r="D9" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E9" s="13">
         <v>0.7</v>
@@ -1040,8 +1043,8 @@
       <c r="C10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>80</v>
+      <c r="D10" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E10" s="13">
         <v>2.7</v>
@@ -1058,8 +1061,8 @@
       <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>80</v>
+      <c r="D11" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E11" s="13">
         <v>3</v>
@@ -1074,10 +1077,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>80</v>
+        <v>55</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E12" s="13">
         <v>0.8</v>
@@ -1086,16 +1089,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>65</v>
-      </c>
       <c r="C13" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E13" s="19">
         <v>0.6</v>
@@ -1104,16 +1107,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="19">
         <v>0.6</v>
@@ -1122,16 +1125,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="19">
         <v>0.6</v>
@@ -1140,16 +1143,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>71</v>
-      </c>
       <c r="C16" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" s="19">
         <v>0.6</v>
@@ -1158,16 +1161,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>73</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="19">
         <v>0.6</v>
@@ -1176,16 +1179,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>75</v>
-      </c>
       <c r="C18" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E18" s="19">
         <v>0.6</v>
@@ -1194,16 +1197,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="19">
         <v>7</v>
@@ -1222,7 +1225,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1246,7 +1249,7 @@
         <v>31</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>32</v>
@@ -1263,10 +1266,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E2" s="26">
         <v>0</v>
@@ -1284,7 +1287,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="29">
         <v>0.8</v>
@@ -1302,7 +1305,7 @@
         <v>41</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="29">
         <v>0.6</v>
@@ -1317,10 +1320,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E5" s="29">
         <v>0.8</v>
@@ -1337,8 +1340,8 @@
       <c r="C6" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>80</v>
+      <c r="D6" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E6" s="29">
         <v>0.9</v>
@@ -1355,8 +1358,8 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>80</v>
+      <c r="D7" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E7" s="29">
         <v>0.6</v>
@@ -1373,8 +1376,8 @@
       <c r="C8" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>80</v>
+      <c r="D8" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E8" s="29">
         <v>4</v>
@@ -1391,8 +1394,8 @@
       <c r="C9" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>80</v>
+      <c r="D9" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E9" s="29">
         <v>0.7</v>
@@ -1409,8 +1412,8 @@
       <c r="C10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>80</v>
+      <c r="D10" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E10" s="29">
         <v>2.7</v>
@@ -1427,8 +1430,8 @@
       <c r="C11" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>80</v>
+      <c r="D11" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E11" s="29">
         <v>3</v>
@@ -1443,10 +1446,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>80</v>
+        <v>55</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="E12" s="29">
         <v>0.8</v>
@@ -1455,16 +1458,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="C13" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E13" s="29">
         <v>0.6</v>
@@ -1473,16 +1476,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="29">
         <v>0.6</v>
@@ -1491,16 +1494,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="29">
         <v>0.6</v>
@@ -1509,16 +1512,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>71</v>
-      </c>
       <c r="C16" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" s="29">
         <v>0.6</v>
@@ -1527,16 +1530,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>73</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="29">
         <v>0.6</v>
@@ -1545,16 +1548,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="C18" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E18" s="29">
         <v>0.6</v>
@@ -1563,16 +1566,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>76</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>77</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="29">
         <v>7</v>
@@ -1591,7 +1594,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,7 +1618,7 @@
         <v>33</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>34</v>
@@ -1632,10 +1635,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -1653,7 +1656,7 @@
         <v>37</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="8">
         <v>2.7</v>
@@ -1671,7 +1674,7 @@
         <v>37</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E4" s="8">
         <v>3</v>
@@ -1689,7 +1692,7 @@
         <v>37</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E5" s="6">
         <v>3.2</v>
@@ -1707,7 +1710,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E6" s="8">
         <v>2.8</v>
@@ -1722,20 +1725,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.54296875" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1745,14 +1749,17 @@
       <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1760,14 +1767,17 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="4">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1777,12 +1787,15 @@
       <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="4">
         <v>0.99</v>
       </c>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1792,10 +1805,13 @@
       <c r="C4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4">
         <v>0.99</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1807,7 +1823,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1842,7 +1858,7 @@
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2">
         <v>1.06</v>
@@ -1855,7 +1871,7 @@
         <v>1.6860067999999999E-2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1877,7 +1893,7 @@
         <v>0.22000000000000003</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1919,7 +1935,7 @@
         <v>8.320000000000001E-2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1942,7 +1958,7 @@
         <v>0.20800000000000002</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1964,15 +1980,15 @@
         <v>0.20800000000000002</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="C8" s="2">
         <v>0.29899999999999999</v>
@@ -1986,15 +2002,15 @@
         <v>0.35360000000000003</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="21">
         <v>5.3999999999999999E-2</v>

</xml_diff>

<commit_message>
updating with none value
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -1829,10 +1829,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,176 +1862,194 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="21">
+        <v>0</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="2">
         <v>1.06</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="2">
         <f>0.228/3.6</f>
         <v>6.3333333333333339E-2</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
         <v>1.6860067999999999E-2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C4" s="6">
         <v>2.52</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D4" s="6">
         <f>0.102/3.6</f>
         <v>2.8333333333333332E-2</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E4" s="10">
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>1.23</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <f>0.301/3.6</f>
         <v>8.3611111111111108E-2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <f>(1.2+1.45)/2</f>
         <v>1.325</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <f>((0.399+0.439)/2)/3.6</f>
         <v>0.1163888888888889</v>
-      </c>
-      <c r="E6" s="2">
-        <f>0.2*1.04</f>
-        <v>0.20800000000000002</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="D7" s="2">
-        <f>0.027/3.6</f>
-        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E7" s="2">
         <f>0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D8" s="2">
+        <f>0.027/3.6</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E8" s="2">
+        <f>0.2*1.04</f>
+        <v>0.20800000000000002</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>0.29899999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <f>0.13/3.6</f>
         <v>3.6111111111111115E-2</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E9" s="21">
         <f>0.34*1.04</f>
         <v>0.35360000000000003</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B10" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C10" s="21">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D10" s="21">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E10" s="21">
         <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LCA database Reference documentation update
-updated reference for LCA-infrastructure for SG (Resource)
-updated missing reference for LCA-infrastructure for CH (Resource - Solid Waste)
- PEN and CO2 are from ecoinvent 3.4 (SG), KBOB (CH)
- costs are calculated from CEA
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\Github\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="DHW" sheetId="4" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Natural Gas</t>
   </si>
   <si>
-    <t>from CEA, costs in USD-2015,</t>
-  </si>
-  <si>
     <t>Electricity</t>
   </si>
   <si>
@@ -261,24 +258,6 @@
     <t>BIOGAS</t>
   </si>
   <si>
-    <t>KBOB 2009/1:2016, ID 41.004/41.005 (average)</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.006 Stückholz (average)</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.009 Biogas</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.002 Erdgas</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix</t>
-  </si>
-  <si>
-    <t>KBOB 2009/1:2016, ID 41.001 Heizöl</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
@@ -355,6 +334,30 @@
   </si>
   <si>
     <t>scale_el</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 42.001 Kehrichtverbrennung, cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.002 Erdgas, cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 45.020 CH-Verbrauchermix, cost from CEA</t>
+  </si>
+  <si>
+    <t>from CEA, costs in USD-2015, cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.001 Heizöl, cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.004/41.005 (average), cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.006 Stückholz (average), cost from CEA</t>
+  </si>
+  <si>
+    <t>KBOB 2009/1:2016, ID 41.009 Biogas, cost from CEA, cost from CEA</t>
   </si>
 </sst>
 </file>
@@ -441,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -472,7 +475,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,7 +510,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -861,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,13 +873,12 @@
     <col min="1" max="1" width="69.28515625" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="19" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -888,17 +888,14 @@
       <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>84</v>
+      <c r="D1" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -906,17 +903,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="E2" s="9">
         <v>0</v>
       </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -926,15 +922,14 @@
       <c r="C3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="12">
         <v>0.8</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -944,15 +939,14 @@
       <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="D4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="12">
         <v>0.6</v>
       </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -960,17 +954,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="13">
+        <v>70</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="12">
         <v>0.8</v>
       </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -980,15 +973,14 @@
       <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="D6" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="12">
         <v>0.9</v>
       </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -998,15 +990,14 @@
       <c r="C7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="D7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="12">
         <v>0.6</v>
       </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1016,15 +1007,14 @@
       <c r="C8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="D8" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="12">
         <v>4</v>
       </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1032,17 +1022,16 @@
         <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="13">
+        <v>50</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="12">
         <v>0.7</v>
       </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -1052,15 +1041,14 @@
       <c r="C10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="12">
         <v>2.7</v>
       </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1070,15 +1058,14 @@
       <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="D11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="12">
         <v>3</v>
       </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1086,141 +1073,133 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="13">
+        <v>54</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="12">
         <v>0.8</v>
       </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="C16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="19">
+      <c r="B17" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="18">
         <v>0.6</v>
       </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="15" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="B18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="D19" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="F18" s="28"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="19">
+      <c r="E19" s="18">
         <v>7</v>
       </c>
-      <c r="F19" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1231,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,12 +1221,11 @@
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="19" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1257,339 +1235,318 @@
       <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>85</v>
+      <c r="D1" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="27">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="26">
-        <v>0</v>
-      </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="B16" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="27">
         <v>7</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="29">
-        <v>0.9</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="29">
-        <v>4</v>
-      </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="29">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="29">
-        <v>2.7</v>
-      </c>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="29">
-        <v>3</v>
-      </c>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12" s="29">
-        <v>0.8</v>
-      </c>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="29">
-        <v>0.6</v>
-      </c>
-      <c r="F18" s="28"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="29">
-        <v>7</v>
-      </c>
-      <c r="F19" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1600,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,12 +1568,11 @@
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="19" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1626,17 +1582,14 @@
       <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>86</v>
+      <c r="D1" s="20" t="s">
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1644,17 +1597,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>55</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1664,15 +1616,14 @@
       <c r="C3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>80</v>
+      <c r="D3" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="E3" s="8">
         <v>2.7</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1682,15 +1633,14 @@
       <c r="C4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>80</v>
+      <c r="D4" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="E4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1700,15 +1650,14 @@
       <c r="C5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="24" t="s">
-        <v>81</v>
+      <c r="D5" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="E5" s="6">
         <v>3.2</v>
       </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -1718,13 +1667,12 @@
       <c r="C6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>81</v>
+      <c r="D6" s="24" t="s">
+        <v>74</v>
       </c>
       <c r="E6" s="8">
         <v>2.8</v>
       </c>
-      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1734,21 +1682,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1758,17 +1705,14 @@
       <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>87</v>
+      <c r="D1" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1776,17 +1720,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -1797,14 +1740,13 @@
         <v>37</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E3" s="4">
         <v>0.99</v>
       </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1812,15 +1754,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E4" s="4">
         <v>0.99</v>
       </c>
-      <c r="F4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1831,15 +1772,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1862,30 +1803,30 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="21">
+      <c r="B2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="20">
         <v>0</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="20">
         <v>0</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>0</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2">
         <v>1.06</v>
@@ -1897,13 +1838,13 @@
       <c r="E3" s="2">
         <v>1.6860067999999999E-2</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>59</v>
+      <c r="F3" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>37</v>
@@ -1919,16 +1860,16 @@
         <f>0.2*1.1</f>
         <v>0.22000000000000003</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>60</v>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C5" s="2">
         <v>1E-4</v>
@@ -1939,13 +1880,13 @@
       <c r="E5" s="2">
         <v>1E-4</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>48</v>
+      <c r="F5" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
@@ -1961,13 +1902,13 @@
         <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>61</v>
+      <c r="F6" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>41</v>
@@ -1984,13 +1925,13 @@
         <f>0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>56</v>
+      <c r="F7" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>42</v>
@@ -2006,16 +1947,16 @@
         <f>0.2*1.04</f>
         <v>0.20800000000000002</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>57</v>
+      <c r="F8" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>83</v>
+      <c r="A9" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2">
         <v>0.29899999999999999</v>
@@ -2024,32 +1965,34 @@
         <f>0.13/3.6</f>
         <v>3.6111111111111115E-2</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <f>0.34*1.04</f>
         <v>0.35360000000000003</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>58</v>
+      <c r="F9" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="21">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="D10" s="21">
-        <v>1E-3</v>
-      </c>
-      <c r="E10" s="21">
+      <c r="A10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="D10" s="20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="20">
         <f>0.08*1.04</f>
         <v>8.320000000000001E-2</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
taking costs out of infrastructure database
</commit_message>
<xml_diff>
--- a/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
+++ b/cea/databases/CH/lifecycle/LCA_infrastructure.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimeno\Documents\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JimenoF\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\lifecycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,25 +123,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Operation costs in US$(2015)/kWh(resource [thermal in case of fuels]).yr</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -228,9 +215,6 @@
   </si>
   <si>
     <t>heatpump - air/air (COP 2.7)</t>
-  </si>
-  <si>
-    <t>costs_kWh</t>
   </si>
   <si>
     <t>district cooling network - air-air</t>
@@ -510,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -531,9 +515,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,9 +555,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +915,7 @@
     <col min="1" max="1" width="69.28515625" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
@@ -950,16 +928,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>43</v>
+      <c r="F1" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,16 +948,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="24">
+        <v>54</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="23">
         <v>0</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>88</v>
+      <c r="F2" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,16 +968,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="25">
+        <v>39</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="24">
         <v>0.8</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>88</v>
+      <c r="F3" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,36 +988,36 @@
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="25">
+        <v>40</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="24">
         <v>0.6</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>88</v>
+      <c r="F4" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="25">
+        <v>69</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="24">
         <v>0.8</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>88</v>
+      <c r="F5" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,16 +1028,16 @@
         <v>9</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="25">
+        <v>36</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="24">
         <v>0.9</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>88</v>
+      <c r="F6" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,16 +1048,16 @@
         <v>10</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="25">
+        <v>41</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="24">
         <v>0.6</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>88</v>
+      <c r="F7" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1090,16 +1068,16 @@
         <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="25">
+        <v>36</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="24">
         <v>4</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>88</v>
+      <c r="F8" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,16 +1088,16 @@
         <v>22</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="25">
+        <v>49</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="24">
         <v>0.7</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>88</v>
+      <c r="F9" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1130,16 +1108,16 @@
         <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="25">
+        <v>36</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="24">
         <v>2.7</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>88</v>
+      <c r="F10" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1150,180 +1128,180 @@
         <v>24</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="25">
+        <v>36</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="24">
         <v>3</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>88</v>
+      <c r="F11" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="12" t="s">
+      <c r="E13" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="B14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="24">
         <v>0.6</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="F14" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="25">
+      <c r="B15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="24">
         <v>0.6</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="F15" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="25">
+      <c r="B16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="24">
         <v>0.6</v>
       </c>
-      <c r="F15" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="F16" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="B17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="24">
         <v>0.6</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="25">
-        <v>2.7</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="12" t="s">
+      <c r="F18" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="B19" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="C19" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="24">
         <v>7</v>
       </c>
-      <c r="F19" s="21" t="s">
-        <v>88</v>
+      <c r="F19" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="26"/>
+      <c r="F20" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
@@ -1345,7 +1323,7 @@
     <col min="1" max="1" width="51" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1358,376 +1336,376 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B5" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="24">
+        <v>4</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="24">
+        <v>3</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="24">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="21" t="s">
+      <c r="B13" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="E13" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="24">
         <v>7</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="25">
-        <v>0.9</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="25">
-        <v>4</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" s="25">
-        <v>0.7</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="25">
-        <v>2.7</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="25">
-        <v>3</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="25">
-        <v>0.8</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="25">
-        <v>2.7</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="25">
-        <v>0.6</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="25">
-        <v>7</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>88</v>
+      <c r="F19" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1728,7 @@
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1763,16 +1741,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>43</v>
+      <c r="F1" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1783,16 +1761,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>88</v>
+      <c r="F2" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,16 +1781,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>73</v>
+        <v>36</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="E3" s="8">
         <v>2.7</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>88</v>
+      <c r="F3" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1823,16 +1801,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>73</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="E4" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>88</v>
+      <c r="F4" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1843,36 +1821,36 @@
         <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>74</v>
+        <v>36</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="E5" s="6">
         <v>3.2</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>88</v>
+      <c r="F5" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>74</v>
+        <v>36</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="E6" s="8">
         <v>2.8</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>88</v>
+      <c r="F6" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1871,7 @@
   <cols>
     <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="15" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1905,16 +1883,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>80</v>
+        <v>35</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,16 +1903,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>88</v>
+      <c r="F2" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,16 +1923,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="4">
         <v>0.99</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>88</v>
+      <c r="F3" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1965,16 +1943,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="4">
         <v>0.99</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>88</v>
+      <c r="F4" s="20" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1984,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,11 +1974,10 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2014,201 +1991,165 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="20">
+      <c r="B2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="19">
         <v>0</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <v>0</v>
       </c>
-      <c r="E2" s="17">
-        <v>0</v>
-      </c>
-      <c r="F2" s="17"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="20">
+        <v>69</v>
+      </c>
+      <c r="C3" s="19">
         <v>1.06</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <f>0.228/3.6</f>
         <v>6.3333333333333339E-2</v>
       </c>
-      <c r="E3" s="20">
-        <v>1.6860067999999999E-2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="20">
+        <v>36</v>
+      </c>
+      <c r="C4" s="19">
         <v>2.52</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
         <f>0.102/3.6</f>
         <v>2.8333333333333332E-2</v>
       </c>
-      <c r="E4" s="9">
-        <f>0.2*1.1</f>
-        <v>0.22000000000000003</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="19">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="20">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="D5" s="20">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="E5" s="27">
-        <v>0.6</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="20">
+        <v>39</v>
+      </c>
+      <c r="C6" s="19">
         <v>1.23</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <f>0.301/3.6</f>
         <v>8.3611111111111108E-2</v>
       </c>
-      <c r="E6" s="2">
-        <f>0.08*1.04</f>
-        <v>8.320000000000001E-2</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="20">
+        <v>40</v>
+      </c>
+      <c r="C7" s="19">
         <f>(1.2+1.45)/2</f>
         <v>1.325</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <f>((0.399+0.439)/2)/3.6</f>
         <v>0.1163888888888889</v>
       </c>
-      <c r="E7" s="2">
-        <f>0.2*1.04</f>
-        <v>0.20800000000000002</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="20">
+        <v>41</v>
+      </c>
+      <c r="C8" s="19">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <f>0.027/3.6</f>
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="E8" s="2">
-        <f>0.2*1.04</f>
-        <v>0.20800000000000002</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="20">
+      <c r="E8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="19">
         <v>0.29899999999999999</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <f>0.13/3.6</f>
         <v>3.6111111111111115E-2</v>
       </c>
-      <c r="E9" s="17">
-        <f>0.34*1.04</f>
-        <v>0.35360000000000003</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="E9" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="20">
+      <c r="C10" s="19">
         <v>0.05</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="19">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="17">
-        <f>0.08*1.04</f>
-        <v>8.320000000000001E-2</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>81</v>
+      <c r="E10" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>